<commit_message>
[Add]_02/SkillPopup 초상화, 아이콘 적용
1. SkillPopup 초상화, 아이콘 적용
</commit_message>
<xml_diff>
--- a/Assets/RawData/DataBase/Excel/DataList.xlsx
+++ b/Assets/RawData/DataBase/Excel/DataList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SkillData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -1304,6 +1304,110 @@
   </si>
   <si>
     <t>Prefabs/Skill/Eve/Skill4</t>
+  </si>
+  <si>
+    <t>IconPath</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill1</t>
+  </si>
+  <si>
+    <t>UI/Icon/Skill1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill2</t>
+  </si>
+  <si>
+    <t>UI/Icon/Skill2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Breesha3</t>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Breesha3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Breesha4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Adam4</t>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Breesha4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Eve3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Eve3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Eve3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Eve4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Eve4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Adam3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Adam3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Adam3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Adam4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Abel3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Abel3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Abel3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Abel4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Abel4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Kain3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Kain3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Skill_Kain4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1764,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N8"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1782,10 +1886,11 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="12" customWidth="1"/>
+    <col min="14" max="14" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="1026" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1825,8 +1930,11 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>101011</v>
       </c>
@@ -1866,8 +1974,11 @@
       <c r="M2" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N2" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>101021</v>
       </c>
@@ -1907,8 +2018,11 @@
       <c r="M3" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N3" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>101031</v>
       </c>
@@ -1948,8 +2062,11 @@
       <c r="M4" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N4" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>101032</v>
       </c>
@@ -1989,8 +2106,11 @@
       <c r="M5" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N5" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>101033</v>
       </c>
@@ -2030,8 +2150,11 @@
       <c r="M6" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N6" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>101041</v>
       </c>
@@ -2071,8 +2194,11 @@
       <c r="M7" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N7" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>101042</v>
       </c>
@@ -2112,8 +2238,11 @@
       <c r="M8" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N8" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>102011</v>
       </c>
@@ -2153,8 +2282,11 @@
       <c r="M9" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N9" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>102021</v>
       </c>
@@ -2194,8 +2326,11 @@
       <c r="M10" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N10" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>102031</v>
       </c>
@@ -2235,8 +2370,11 @@
       <c r="M11" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N11" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>102032</v>
       </c>
@@ -2276,8 +2414,11 @@
       <c r="M12" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N12" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>102033</v>
       </c>
@@ -2317,8 +2458,11 @@
       <c r="M13" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N13" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>102041</v>
       </c>
@@ -2358,8 +2502,11 @@
       <c r="M14" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N14" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>102042</v>
       </c>
@@ -2399,8 +2546,11 @@
       <c r="M15" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N15" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>103011</v>
       </c>
@@ -2440,8 +2590,11 @@
       <c r="M16" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N16" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>103021</v>
       </c>
@@ -2481,8 +2634,11 @@
       <c r="M17" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N17" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>103031</v>
       </c>
@@ -2522,8 +2678,11 @@
       <c r="M18" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N18" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>103032</v>
       </c>
@@ -2563,8 +2722,11 @@
       <c r="M19" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N19" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>103033</v>
       </c>
@@ -2604,8 +2766,11 @@
       <c r="M20" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N20" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>103041</v>
       </c>
@@ -2645,8 +2810,11 @@
       <c r="M21" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N21" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>103042</v>
       </c>
@@ -2686,8 +2854,11 @@
       <c r="M22" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N22" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>104011</v>
       </c>
@@ -2727,8 +2898,11 @@
       <c r="M23" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N23" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>104021</v>
       </c>
@@ -2768,8 +2942,11 @@
       <c r="M24" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N24" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>104031</v>
       </c>
@@ -2809,8 +2986,11 @@
       <c r="M25" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N25" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>104032</v>
       </c>
@@ -2850,8 +3030,11 @@
       <c r="M26" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N26" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>104033</v>
       </c>
@@ -2891,8 +3074,11 @@
       <c r="M27" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N27" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>104041</v>
       </c>
@@ -2932,8 +3118,11 @@
       <c r="M28" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N28" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>104042</v>
       </c>
@@ -2973,8 +3162,11 @@
       <c r="M29" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N29" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>105011</v>
       </c>
@@ -3014,8 +3206,11 @@
       <c r="M30" s="7" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N30" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>105021</v>
       </c>
@@ -3055,8 +3250,11 @@
       <c r="M31" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N31" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>105031</v>
       </c>
@@ -3096,8 +3294,11 @@
       <c r="M32" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N32" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>105032</v>
       </c>
@@ -3137,8 +3338,11 @@
       <c r="M33" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N33" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>105033</v>
       </c>
@@ -3178,8 +3382,11 @@
       <c r="M34" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N34" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>105041</v>
       </c>
@@ -3219,8 +3426,11 @@
       <c r="M35" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N35" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>105042</v>
       </c>
@@ -3260,8 +3470,11 @@
       <c r="M36" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N36" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>106011</v>
       </c>
@@ -3299,8 +3512,11 @@
         <v>1</v>
       </c>
       <c r="M37" s="2"/>
-    </row>
-    <row r="38" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N37" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>106021</v>
       </c>
@@ -3338,8 +3554,11 @@
         <v>0</v>
       </c>
       <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N38" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>106031</v>
       </c>
@@ -3377,8 +3596,9 @@
         <v>2</v>
       </c>
       <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>106032</v>
       </c>
@@ -3416,8 +3636,9 @@
         <v>2</v>
       </c>
       <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>106033</v>
       </c>
@@ -3455,8 +3676,9 @@
         <v>2</v>
       </c>
       <c r="M41" s="2"/>
-    </row>
-    <row r="42" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>106041</v>
       </c>
@@ -3494,8 +3716,9 @@
         <v>-5</v>
       </c>
       <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>106042</v>
       </c>
@@ -3533,6 +3756,7 @@
         <v>-5</v>
       </c>
       <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3545,8 +3769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3615,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="13">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="E2" s="13">
         <v>50</v>

</xml_diff>

<commit_message>
[Addfix]_03/Kana 캐릭터 추가, item아이콘 추가
1. 캐릭터 추가
2. 아이콘 추가
</commit_message>
<xml_diff>
--- a/Assets/RawData/DataBase/Excel/DataList.xlsx
+++ b/Assets/RawData/DataBase/Excel/DataList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterData" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="244">
   <si>
     <t>ID</t>
   </si>
@@ -744,6 +744,66 @@
   </si>
   <si>
     <t>모든 사실을 숨기고 있었던 Dr. 브리샤가 우리의 품으로 돌아왔다.. 그녀가 내뱉은 충격적인 첫 말은…</t>
+  </si>
+  <si>
+    <t>UI/Icon/Skill1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/book</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/book</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/book</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/sword</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/armor</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/hp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/hp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/scroll</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_101</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_102</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_103</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_104</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_105</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/Icon/Portrait_106</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1536,7 +1596,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1651,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -4467,7 +4527,8 @@
     <col min="11" max="12" width="8.6640625" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
-    <col min="15" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="12.6" customHeight="1">
@@ -5012,7 +5073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -5107,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5160,7 +5221,9 @@
       <c r="F2" s="30">
         <v>1</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="30">
@@ -5181,7 +5244,9 @@
       <c r="F3" s="30">
         <v>1</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="32" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="24">
       <c r="A4" s="30">
@@ -5202,7 +5267,9 @@
       <c r="F4" s="30">
         <v>1</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="32" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="A5" s="30">
@@ -5223,7 +5290,9 @@
       <c r="F5" s="30">
         <v>1</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="32" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="A6" s="30">
@@ -5244,7 +5313,9 @@
       <c r="F6" s="30">
         <v>1</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="32" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="24">
       <c r="A7" s="30">
@@ -5265,7 +5336,9 @@
       <c r="F7" s="30">
         <v>1</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="32" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="24">
       <c r="A8" s="30">
@@ -5286,7 +5359,9 @@
       <c r="F8" s="30">
         <v>1</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="30">
@@ -5307,7 +5382,9 @@
       <c r="F9" s="30">
         <v>1</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="32" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="30">
@@ -5328,6 +5405,9 @@
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="G10" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="30">
@@ -5348,6 +5428,9 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="30">
@@ -5368,6 +5451,9 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="30">
@@ -5388,6 +5474,9 @@
       <c r="F13">
         <v>1</v>
       </c>
+      <c r="G13" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="30">
@@ -5408,6 +5497,9 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="G14" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="30">
@@ -5427,6 +5519,9 @@
       </c>
       <c r="F15">
         <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:7">

</xml_diff>

<commit_message>
[Addfix]_04/Skill 쿨타임, Description 표시
</commit_message>
<xml_diff>
--- a/Assets/RawData/DataBase/Excel/DataList.xlsx
+++ b/Assets/RawData/DataBase/Excel/DataList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterData" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="276">
   <si>
     <t>_chapterId</t>
   </si>
@@ -46,9 +46,6 @@
     <t>_stageCount</t>
   </si>
   <si>
-    <t>태초의 푸루샤</t>
-  </si>
-  <si>
     <t>주요 연구의 핵심인 Dr.브리샤를 되찾기 위해 알 수 없는 드론들이 우리들의 본거지를 공격하기 시작했다. 우리의 힘으로 Dr.브리샤와 기지를 지킬 수 있을까?</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
   </si>
   <si>
     <t>UI/Icon/Skill_Kain4</t>
-  </si>
-  <si>
-    <t>대상 1명에게 연발사격 (치명타 시 턴획득 1회)</t>
   </si>
   <si>
     <t>헤드샷 (치확+15%/치피+25퍼)</t>
@@ -872,6 +866,18 @@
   </si>
   <si>
     <t>플레이어 방어력 비례 쉴드 생성</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>태초의 푸루샤</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>에너지를 집중하여 적 대상 1명을 찌른 후 폭발시킨다</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상 1명에게 연발사격</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1501,12 +1507,15 @@
   <dimension ref="A1:AMK8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="1" customWidth="1"/>
+    <col min="4" max="1025" width="14.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
@@ -1528,10 +1537,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
@@ -1542,10 +1551,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="3">
         <v>3</v>
@@ -1556,10 +1565,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
@@ -1570,10 +1579,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
@@ -1584,10 +1593,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1598,10 +1607,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="3">
         <v>3</v>
@@ -1612,10 +1621,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -1632,9 +1641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK51"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1654,52 +1663,52 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1707,49 +1716,49 @@
         <v>101011</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>1</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7">
-        <v>0</v>
-      </c>
-      <c r="K2" s="7">
-        <v>0</v>
-      </c>
-      <c r="L2" s="7">
-        <v>1</v>
-      </c>
-      <c r="M2" s="7">
-        <v>0</v>
-      </c>
-      <c r="N2" s="7">
-        <v>1</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1757,10 +1766,10 @@
         <v>101021</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D3" s="9">
         <v>2</v>
@@ -1796,10 +1805,10 @@
         <v>0</v>
       </c>
       <c r="O3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1807,10 +1816,10 @@
         <v>101031</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
@@ -1846,10 +1855,10 @@
         <v>2</v>
       </c>
       <c r="O4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1857,10 +1866,10 @@
         <v>101032</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
@@ -1896,10 +1905,10 @@
         <v>2</v>
       </c>
       <c r="O5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1907,10 +1916,10 @@
         <v>101033</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
@@ -1946,10 +1955,10 @@
         <v>2</v>
       </c>
       <c r="O6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1957,10 +1966,10 @@
         <v>101041</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D7" s="11">
         <v>1</v>
@@ -1996,10 +2005,10 @@
         <v>-5</v>
       </c>
       <c r="O7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2007,10 +2016,10 @@
         <v>101042</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11">
         <v>1</v>
@@ -2046,10 +2055,10 @@
         <v>-5</v>
       </c>
       <c r="O8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2057,11 +2066,11 @@
         <v>102011</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="D9" s="13">
         <v>0</v>
       </c>
@@ -2096,10 +2105,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2107,10 +2116,10 @@
         <v>102021</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D10" s="9">
         <v>2</v>
@@ -2146,10 +2155,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2157,10 +2166,10 @@
         <v>102031</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -2196,10 +2205,10 @@
         <v>4</v>
       </c>
       <c r="O11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2207,10 +2216,10 @@
         <v>102032</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -2246,10 +2255,10 @@
         <v>4</v>
       </c>
       <c r="O12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2257,10 +2266,10 @@
         <v>102033</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
@@ -2296,10 +2305,10 @@
         <v>4</v>
       </c>
       <c r="O13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2307,10 +2316,10 @@
         <v>102041</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
@@ -2346,10 +2355,10 @@
         <v>-5</v>
       </c>
       <c r="O14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2357,10 +2366,10 @@
         <v>102042</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="15">
         <v>1</v>
@@ -2396,10 +2405,10 @@
         <v>-5</v>
       </c>
       <c r="O15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2407,11 +2416,11 @@
         <v>103011</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="D16" s="7">
         <v>0</v>
       </c>
@@ -2446,10 +2455,10 @@
         <v>1</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2457,10 +2466,10 @@
         <v>103021</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
@@ -2496,10 +2505,10 @@
         <v>0</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2507,10 +2516,10 @@
         <v>103031</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -2546,10 +2555,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2557,10 +2566,10 @@
         <v>103032</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
@@ -2596,10 +2605,10 @@
         <v>2</v>
       </c>
       <c r="O19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P19" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2607,10 +2616,10 @@
         <v>103033</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
@@ -2646,10 +2655,10 @@
         <v>2</v>
       </c>
       <c r="O20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P20" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="P20" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2657,10 +2666,10 @@
         <v>103041</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>64</v>
+        <v>274</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
@@ -2696,10 +2705,10 @@
         <v>-5</v>
       </c>
       <c r="O21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P21" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2707,10 +2716,10 @@
         <v>103042</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
@@ -2746,10 +2755,10 @@
         <v>-5</v>
       </c>
       <c r="O22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2757,10 +2766,10 @@
         <v>104011</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="18">
         <v>0</v>
@@ -2796,10 +2805,10 @@
         <v>1</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2807,10 +2816,10 @@
         <v>104021</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D24" s="9">
         <v>2</v>
@@ -2846,10 +2855,10 @@
         <v>0</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2857,10 +2866,10 @@
         <v>104031</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="7">
         <v>3</v>
@@ -2896,10 +2905,10 @@
         <v>2</v>
       </c>
       <c r="O25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P25" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2907,10 +2916,10 @@
         <v>104032</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="7">
         <v>3</v>
@@ -2946,10 +2955,10 @@
         <v>2</v>
       </c>
       <c r="O26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="P26" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2957,10 +2966,10 @@
         <v>104033</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="7">
         <v>3</v>
@@ -2996,10 +3005,10 @@
         <v>2</v>
       </c>
       <c r="O27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P27" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="P27" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -3007,10 +3016,10 @@
         <v>104041</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="9">
         <v>4</v>
@@ -3046,10 +3055,10 @@
         <v>-5</v>
       </c>
       <c r="O28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="P28" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="P28" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -3057,10 +3066,10 @@
         <v>104042</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="9">
         <v>4</v>
@@ -3096,10 +3105,10 @@
         <v>-5</v>
       </c>
       <c r="O29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="P29" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -3107,10 +3116,10 @@
         <v>105011</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="18">
         <v>0</v>
@@ -3146,10 +3155,10 @@
         <v>1</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -3157,10 +3166,10 @@
         <v>105021</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D31" s="9">
         <v>2</v>
@@ -3196,10 +3205,10 @@
         <v>0</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P31" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -3207,10 +3216,10 @@
         <v>105031</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="11">
         <v>0</v>
@@ -3246,10 +3255,10 @@
         <v>2</v>
       </c>
       <c r="O32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P32" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="P32" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -3257,10 +3266,10 @@
         <v>105032</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="11">
         <v>0</v>
@@ -3296,10 +3305,10 @@
         <v>2</v>
       </c>
       <c r="O33" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P33" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="P33" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -3307,10 +3316,10 @@
         <v>105033</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="11">
         <v>0</v>
@@ -3346,10 +3355,10 @@
         <v>2</v>
       </c>
       <c r="O34" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -3357,10 +3366,10 @@
         <v>105041</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D35" s="7">
         <v>0</v>
@@ -3396,10 +3405,10 @@
         <v>-5</v>
       </c>
       <c r="O35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P35" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="P35" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3407,10 +3416,10 @@
         <v>105042</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D36" s="15">
         <v>0</v>
@@ -3446,10 +3455,10 @@
         <v>-5</v>
       </c>
       <c r="O36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="P36" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="P36" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3457,11 +3466,11 @@
         <v>106011</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="D37" s="7">
         <v>0</v>
       </c>
@@ -3496,10 +3505,10 @@
         <v>1</v>
       </c>
       <c r="O37" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3507,10 +3516,10 @@
         <v>106021</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D38" s="9">
         <v>2</v>
@@ -3546,10 +3555,10 @@
         <v>0</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3557,10 +3566,10 @@
         <v>106031</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>87</v>
+        <v>275</v>
       </c>
       <c r="D39" s="7">
         <v>0</v>
@@ -3596,10 +3605,10 @@
         <v>2</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -3607,10 +3616,10 @@
         <v>106032</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>275</v>
       </c>
       <c r="D40" s="7">
         <v>0</v>
@@ -3646,10 +3655,10 @@
         <v>2</v>
       </c>
       <c r="O40" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="P40" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="P40" s="8" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3657,10 +3666,10 @@
         <v>106033</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>87</v>
+        <v>275</v>
       </c>
       <c r="D41" s="7">
         <v>0</v>
@@ -3696,10 +3705,10 @@
         <v>2</v>
       </c>
       <c r="O41" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="P41" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="P41" s="8" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3707,10 +3716,10 @@
         <v>106041</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D42" s="7">
         <v>0</v>
@@ -3746,10 +3755,10 @@
         <v>-5</v>
       </c>
       <c r="O42" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="P42" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="P42" s="8" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3757,10 +3766,10 @@
         <v>106042</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D43" s="15">
         <v>0</v>
@@ -3796,10 +3805,10 @@
         <v>-5</v>
       </c>
       <c r="O43" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="P43" s="16" t="s">
         <v>257</v>
-      </c>
-      <c r="P43" s="16" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3807,10 +3816,10 @@
         <v>101001011</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" s="7">
         <v>0</v>
@@ -3846,7 +3855,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P44" s="8"/>
     </row>
@@ -3855,10 +3864,10 @@
         <v>101001021</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D45" s="20">
         <v>0</v>
@@ -3894,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P45" s="21"/>
     </row>
@@ -3903,10 +3912,10 @@
         <v>101002011</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D46" s="7">
         <v>0</v>
@@ -3942,7 +3951,7 @@
         <v>0</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P46" s="8"/>
     </row>
@@ -3951,10 +3960,10 @@
         <v>101002021</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D47" s="20">
         <v>0</v>
@@ -3990,7 +3999,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P47" s="21"/>
     </row>
@@ -3999,10 +4008,10 @@
         <v>101003011</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D48" s="7">
         <v>0</v>
@@ -4038,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="O48" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P48" s="8"/>
     </row>
@@ -4047,10 +4056,10 @@
         <v>101003021</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="15">
         <v>1</v>
@@ -4086,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P49" s="16"/>
     </row>
@@ -4095,10 +4104,10 @@
         <v>201001011</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D50" s="7">
         <v>0</v>
@@ -4134,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P50" s="8"/>
     </row>
@@ -4143,10 +4152,10 @@
         <v>201001021</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" s="20">
         <v>1</v>
@@ -4182,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P51" s="21"/>
     </row>
@@ -4197,7 +4206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -4212,25 +4221,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4248,7 +4257,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="26">
         <v>0</v>
@@ -4263,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4271,7 +4280,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="26">
         <v>0</v>
@@ -4286,7 +4295,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4294,7 +4303,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="26">
         <v>0</v>
@@ -4309,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4317,7 +4326,7 @@
         <v>201</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="26">
         <v>0</v>
@@ -4332,7 +4341,7 @@
         <v>0.7</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4340,7 +4349,7 @@
         <v>202</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" s="26">
         <v>0</v>
@@ -4355,7 +4364,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4363,7 +4372,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8" s="26">
         <v>0</v>
@@ -4378,7 +4387,7 @@
         <v>0.7</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4386,7 +4395,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -4401,7 +4410,7 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4409,7 +4418,7 @@
         <v>205</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
@@ -4424,7 +4433,7 @@
         <v>0.2</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4432,7 +4441,7 @@
         <v>206</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
@@ -4447,7 +4456,7 @@
         <v>0.3</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
@@ -4455,7 +4464,7 @@
         <v>207</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -4470,7 +4479,7 @@
         <v>0.6</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
@@ -4478,7 +4487,7 @@
         <v>208</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
@@ -4493,7 +4502,7 @@
         <v>0.8</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
@@ -4501,7 +4510,7 @@
         <v>209</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" s="26">
         <v>0</v>
@@ -4516,7 +4525,7 @@
         <v>0.9</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4554,43 +4563,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="12.75">
       <c r="A1" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="M1" s="29" t="s">
         <v>135</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75">
@@ -4598,7 +4607,7 @@
         <v>101001</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="30">
         <v>1</v>
@@ -4628,7 +4637,7 @@
         <v>100</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M2" s="31"/>
     </row>
@@ -4637,7 +4646,7 @@
         <v>101002</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="30">
         <v>3</v>
@@ -4667,7 +4676,7 @@
         <v>200</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M3" s="31"/>
     </row>
@@ -4676,7 +4685,7 @@
         <v>101003</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="30">
         <v>5</v>
@@ -4706,7 +4715,7 @@
         <v>300</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M4" s="31"/>
     </row>
@@ -4715,7 +4724,7 @@
         <v>201001</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="30">
         <v>10</v>
@@ -4745,7 +4754,7 @@
         <v>300</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M5" s="31"/>
     </row>
@@ -4784,49 +4793,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="12.6" customHeight="1">
       <c r="A1" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="F1" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="H1" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="33" t="s">
-        <v>136</v>
-      </c>
       <c r="O1" s="33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P1" s="33"/>
     </row>
@@ -4835,7 +4844,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="33">
         <v>3000</v>
@@ -4871,10 +4880,10 @@
         <v>1.05</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P2" s="35"/>
     </row>
@@ -4883,7 +4892,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="33">
         <v>2500</v>
@@ -4919,10 +4928,10 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P3" s="35"/>
     </row>
@@ -4931,7 +4940,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="33">
         <v>2500</v>
@@ -4967,10 +4976,10 @@
         <v>1.3</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P4" s="35"/>
     </row>
@@ -4979,7 +4988,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="33">
         <v>2000</v>
@@ -5015,10 +5024,10 @@
         <v>1.45</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P5" s="35"/>
     </row>
@@ -5027,7 +5036,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="33">
         <v>2000</v>
@@ -5063,10 +5072,10 @@
         <v>1.2</v>
       </c>
       <c r="N6" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P6" s="35"/>
     </row>
@@ -5075,7 +5084,7 @@
         <v>106</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="33">
         <v>4000</v>
@@ -5111,10 +5120,10 @@
         <v>0.8</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P7" s="35"/>
     </row>
@@ -5130,17 +5139,17 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
@@ -5152,66 +5161,68 @@
     <col min="15" max="15" width="19.5" customWidth="1"/>
     <col min="16" max="16" width="15.6640625" customWidth="1"/>
     <col min="17" max="17" width="19.5" customWidth="1"/>
-    <col min="18" max="1025" width="11" customWidth="1"/>
+    <col min="18" max="18" width="16.5" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="20" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="Q1" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>182</v>
-      </c>
       <c r="S1" s="33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.6" customHeight="1">
@@ -5219,7 +5230,7 @@
         <v>110101</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="33">
         <v>101001</v>
@@ -5256,7 +5267,7 @@
         <v>110102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="33">
         <v>101001</v>
@@ -5272,10 +5283,18 @@
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
       <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
+      <c r="M3" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N3" s="33">
+        <v>1</v>
+      </c>
+      <c r="O3" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P3" s="33">
+        <v>3</v>
+      </c>
       <c r="Q3" s="35"/>
       <c r="R3" s="35"/>
       <c r="S3" s="35"/>
@@ -5285,7 +5304,7 @@
         <v>110103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4" s="35">
         <v>101002</v>
@@ -5305,10 +5324,18 @@
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="M4" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N4" s="33">
+        <v>2</v>
+      </c>
+      <c r="O4" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P4" s="33">
+        <v>5</v>
+      </c>
       <c r="Q4" s="35"/>
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
@@ -5318,7 +5345,7 @@
         <v>110201</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" s="35">
         <v>101002</v>
@@ -5331,6 +5358,18 @@
       </c>
       <c r="F5">
         <v>2</v>
+      </c>
+      <c r="M5" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N5" s="33">
+        <v>1</v>
+      </c>
+      <c r="O5" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P5" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="24">
@@ -5338,13 +5377,25 @@
         <v>110202</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6">
         <v>101002</v>
       </c>
       <c r="D6">
         <v>2</v>
+      </c>
+      <c r="M6" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N6" s="33">
+        <v>1</v>
+      </c>
+      <c r="O6" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P6" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
@@ -5352,13 +5403,25 @@
         <v>110203</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7">
         <v>101002</v>
       </c>
       <c r="D7">
         <v>3</v>
+      </c>
+      <c r="M7" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N7" s="33">
+        <v>2</v>
+      </c>
+      <c r="O7" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P7" s="33">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
@@ -5366,13 +5429,25 @@
         <v>110301</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C8">
         <v>101001</v>
       </c>
       <c r="D8">
         <v>2</v>
+      </c>
+      <c r="M8" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N8" s="33">
+        <v>1</v>
+      </c>
+      <c r="O8" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P8" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
@@ -5380,12 +5455,24 @@
         <v>110302</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C9">
         <v>101001</v>
       </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="M9" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N9" s="33">
+        <v>1</v>
+      </c>
+      <c r="O9" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P9" s="33">
         <v>3</v>
       </c>
     </row>
@@ -5394,12 +5481,24 @@
         <v>110303</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C10">
         <v>101001</v>
       </c>
       <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="M10" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N10" s="33">
+        <v>2</v>
+      </c>
+      <c r="O10" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P10" s="33">
         <v>5</v>
       </c>
     </row>
@@ -5408,13 +5507,25 @@
         <v>120101</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C11">
         <v>101001</v>
       </c>
       <c r="D11">
         <v>2</v>
+      </c>
+      <c r="M11" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N11" s="33">
+        <v>1</v>
+      </c>
+      <c r="O11" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P11" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="24">
@@ -5422,12 +5533,24 @@
         <v>120102</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12">
         <v>101001</v>
       </c>
       <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="M12" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N12" s="33">
+        <v>1</v>
+      </c>
+      <c r="O12" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P12" s="33">
         <v>3</v>
       </c>
     </row>
@@ -5436,12 +5559,24 @@
         <v>120103</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13">
         <v>101001</v>
       </c>
       <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="M13" s="33">
+        <v>10401</v>
+      </c>
+      <c r="N13" s="33">
+        <v>2</v>
+      </c>
+      <c r="O13" s="33">
+        <v>10101</v>
+      </c>
+      <c r="P13" s="33">
         <v>5</v>
       </c>
     </row>
@@ -5450,7 +5585,7 @@
         <v>120201</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C14">
         <v>101001</v>
@@ -5464,7 +5599,7 @@
         <v>120202</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C15">
         <v>101001</v>
@@ -5478,7 +5613,7 @@
         <v>120203</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C16">
         <v>101001</v>
@@ -5492,7 +5627,7 @@
         <v>120301</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17">
         <v>101001</v>
@@ -5506,7 +5641,7 @@
         <v>120302</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C18">
         <v>101001</v>
@@ -5520,7 +5655,7 @@
         <v>120303</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C19">
         <v>101001</v>
@@ -5534,7 +5669,7 @@
         <v>130101</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C20">
         <v>101001</v>
@@ -5548,7 +5683,7 @@
         <v>130102</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C21">
         <v>101001</v>
@@ -5562,7 +5697,7 @@
         <v>130103</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C22">
         <v>101001</v>
@@ -5576,7 +5711,7 @@
         <v>130201</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C23">
         <v>101001</v>
@@ -5590,7 +5725,7 @@
         <v>130202</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C24">
         <v>101001</v>
@@ -5604,7 +5739,7 @@
         <v>130203</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C25">
         <v>101001</v>
@@ -5618,7 +5753,7 @@
         <v>130301</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C26">
         <v>101001</v>
@@ -5632,7 +5767,7 @@
         <v>130302</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27">
         <v>101001</v>
@@ -5646,7 +5781,7 @@
         <v>130303</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28">
         <v>101001</v>
@@ -5660,7 +5795,7 @@
         <v>140101</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29">
         <v>101001</v>
@@ -5674,7 +5809,7 @@
         <v>140102</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C30">
         <v>101001</v>
@@ -5688,7 +5823,7 @@
         <v>140103</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C31">
         <v>101001</v>
@@ -5702,7 +5837,7 @@
         <v>140201</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C32">
         <v>101001</v>
@@ -5716,7 +5851,7 @@
         <v>140202</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C33">
         <v>101001</v>
@@ -5730,7 +5865,7 @@
         <v>140203</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C34">
         <v>101001</v>
@@ -5744,7 +5879,7 @@
         <v>140301</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C35">
         <v>101001</v>
@@ -5758,7 +5893,7 @@
         <v>140302</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C36">
         <v>101001</v>
@@ -5772,7 +5907,7 @@
         <v>140303</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C37">
         <v>101001</v>
@@ -5786,7 +5921,7 @@
         <v>150101</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C38">
         <v>101001</v>
@@ -5800,7 +5935,7 @@
         <v>150102</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C39">
         <v>101001</v>
@@ -5814,7 +5949,7 @@
         <v>150103</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C40">
         <v>101001</v>
@@ -5828,7 +5963,7 @@
         <v>150201</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C41">
         <v>101001</v>
@@ -5842,7 +5977,7 @@
         <v>150202</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C42">
         <v>101001</v>
@@ -5856,7 +5991,7 @@
         <v>150203</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C43">
         <v>101001</v>
@@ -5870,7 +6005,7 @@
         <v>150301</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44">
         <v>101001</v>
@@ -5884,7 +6019,7 @@
         <v>150302</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C45">
         <v>101001</v>
@@ -5898,7 +6033,7 @@
         <v>150303</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C46">
         <v>101001</v>
@@ -5923,7 +6058,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -5936,22 +6071,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.5">
       <c r="A1" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="F1" s="36" t="s">
         <v>188</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5">
@@ -5959,10 +6094,10 @@
         <v>1101</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="37">
         <v>110101</v>
@@ -5979,10 +6114,10 @@
         <v>1102</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D3" s="39">
         <v>110201</v>
@@ -5999,10 +6134,10 @@
         <v>1103</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="39">
         <v>110301</v>
@@ -6019,10 +6154,10 @@
         <v>1201</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D5" s="37">
         <v>120101</v>
@@ -6039,10 +6174,10 @@
         <v>1202</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D6" s="39">
         <v>120201</v>
@@ -6059,10 +6194,10 @@
         <v>1203</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" s="39">
         <v>120301</v>
@@ -6079,10 +6214,10 @@
         <v>1301</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D8" s="37">
         <v>130101</v>
@@ -6099,10 +6234,10 @@
         <v>1302</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D9" s="39">
         <v>130201</v>
@@ -6119,10 +6254,10 @@
         <v>1303</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D10" s="39">
         <v>130301</v>
@@ -6139,10 +6274,10 @@
         <v>1401</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D11" s="37">
         <v>140101</v>
@@ -6159,10 +6294,10 @@
         <v>1402</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D12" s="39">
         <v>140201</v>
@@ -6179,10 +6314,10 @@
         <v>1403</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D13" s="39">
         <v>140301</v>
@@ -6199,10 +6334,10 @@
         <v>1501</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D14" s="37">
         <v>150101</v>
@@ -6219,10 +6354,10 @@
         <v>1502</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D15" s="39">
         <v>150201</v>
@@ -6239,10 +6374,10 @@
         <v>1503</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D16" s="39">
         <v>150301</v>
@@ -6259,10 +6394,10 @@
         <v>1601</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D17" s="37">
         <v>160101</v>
@@ -6302,25 +6437,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24">
       <c r="A1" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>211</v>
-      </c>
       <c r="G1" s="33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24">
@@ -6328,13 +6463,13 @@
         <v>10101</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>214</v>
       </c>
       <c r="E2" s="33">
         <v>20</v>
@@ -6343,7 +6478,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24">
@@ -6351,13 +6486,13 @@
         <v>10102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E3" s="33">
         <v>50</v>
@@ -6366,7 +6501,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24">
@@ -6374,13 +6509,13 @@
         <v>10103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" s="33">
         <v>100</v>
@@ -6389,7 +6524,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24">
@@ -6397,22 +6532,22 @@
         <v>10201</v>
       </c>
       <c r="B5" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="E5" s="33">
+        <v>1</v>
+      </c>
+      <c r="F5" s="33">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>221</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="33">
-        <v>1</v>
-      </c>
-      <c r="F5" s="33">
-        <v>1</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24">
@@ -6420,22 +6555,22 @@
         <v>10301</v>
       </c>
       <c r="B6" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="E6" s="33">
+        <v>1</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>225</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="33">
-        <v>1</v>
-      </c>
-      <c r="F6" s="33">
-        <v>1</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24">
@@ -6443,13 +6578,13 @@
         <v>10401</v>
       </c>
       <c r="B7" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>230</v>
       </c>
       <c r="E7" s="33">
         <v>50</v>
@@ -6458,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24">
@@ -6466,13 +6601,13 @@
         <v>10402</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E8" s="33">
         <v>150</v>
@@ -6481,7 +6616,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6489,22 +6624,22 @@
         <v>10501</v>
       </c>
       <c r="B9" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="E9" s="33">
+        <v>1</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+      <c r="G9" s="35" t="s">
         <v>235</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="E9" s="33">
-        <v>1</v>
-      </c>
-      <c r="F9" s="33">
-        <v>1</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6512,13 +6647,13 @@
         <v>10601</v>
       </c>
       <c r="B10" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" t="s">
         <v>238</v>
-      </c>
-      <c r="C10" t="s">
-        <v>239</v>
-      </c>
-      <c r="D10" t="s">
-        <v>240</v>
       </c>
       <c r="E10" s="33">
         <v>101</v>
@@ -6527,7 +6662,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6535,13 +6670,13 @@
         <v>10602</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E11" s="33">
         <v>102</v>
@@ -6550,7 +6685,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6558,13 +6693,13 @@
         <v>10603</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E12" s="33">
         <v>103</v>
@@ -6573,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6581,13 +6716,13 @@
         <v>10604</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E13" s="33">
         <v>104</v>
@@ -6596,7 +6731,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6604,13 +6739,13 @@
         <v>10605</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E14" s="33">
         <v>105</v>
@@ -6619,7 +6754,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6627,13 +6762,13 @@
         <v>10606</v>
       </c>
       <c r="B15" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E15" s="33">
         <v>106</v>
@@ -6642,7 +6777,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6650,10 +6785,10 @@
         <v>10701</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -6685,10 +6820,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
[Fix] 공격버튼 Interactible로 변경
</commit_message>
<xml_diff>
--- a/Assets/RawData/DataBase/Excel/DataList.xlsx
+++ b/Assets/RawData/DataBase/Excel/DataList.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="280">
   <si>
     <t>_chapterId</t>
   </si>
@@ -151,9 +151,6 @@
     <t>쉴드</t>
   </si>
   <si>
-    <t>플레이어 방어력 비례 쉴드 생성</t>
-  </si>
-  <si>
     <t>Prefabs/Skill/Breesha/Skill2</t>
   </si>
   <si>
@@ -310,25 +307,16 @@
     <t>Prefabs/Skill/Kana/Skill2</t>
   </si>
   <si>
-    <t>대상 1명에게 연발사격 (치명타 시 턴획득 1회)</t>
-  </si>
-  <si>
     <t>Prefabs/Skill/Kana/Skill3</t>
   </si>
   <si>
     <t>UI/Icon/Skill_Kana3</t>
   </si>
   <si>
-    <t>헤드샷 (치확+15%/치피+25퍼)</t>
-  </si>
-  <si>
     <t>Prefabs/Skill/Kana/Skill4</t>
   </si>
   <si>
     <t>UI/Icon/Skill_Kana4</t>
-  </si>
-  <si>
-    <t>헤드샷 (치확+20%/치피+40퍼)</t>
   </si>
   <si>
     <t>적 1명 사격</t>
@@ -849,6 +837,52 @@
   </si>
   <si>
     <t>Prefabs/Map/Chapter7/Chap7-3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>궁극(레벨1)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>고유스킬</t>
+  </si>
+  <si>
+    <t>고유스킬</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군 팀 전원 쉴드</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군 팀 전원 행동게이지 +20</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군 전체 공격력 증가</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>적 전체 공격력 감소</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>적 전체 방어력 감소</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군 전체 방어력 증가</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상 1명에게 사격 (치명타 시 턴획득 1회)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상 1명에게 강력한 공격</t>
+  </si>
+  <si>
+    <t>대상 1명에게 강력한 공격</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1609,8 +1643,8 @@
   <dimension ref="A1:AMK53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1733,49 +1767,49 @@
         <v>101021</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>38</v>
+        <v>270</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>102</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>101</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
-        <v>1</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1783,49 +1817,49 @@
         <v>101031</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0</v>
-      </c>
-      <c r="N4" s="7">
-        <v>2</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1833,49 +1867,49 @@
         <v>101032</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>2</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7">
-        <v>0</v>
-      </c>
-      <c r="N5" s="7">
-        <v>2</v>
-      </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1883,49 +1917,49 @@
         <v>101033</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>2</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1933,10 +1967,10 @@
         <v>101041</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="D7" s="11">
         <v>1</v>
@@ -1972,10 +2006,10 @@
         <v>-5</v>
       </c>
       <c r="O7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1983,10 +2017,10 @@
         <v>101042</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="11">
         <v>1</v>
@@ -2022,10 +2056,10 @@
         <v>-5</v>
       </c>
       <c r="O8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2072,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P9" s="14" t="s">
         <v>37</v>
@@ -2083,10 +2117,10 @@
         <v>102021</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>269</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="D10" s="9">
         <v>2</v>
@@ -2095,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="9">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="G10" s="9">
         <v>0</v>
@@ -2122,10 +2156,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2133,10 +2167,10 @@
         <v>102031</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -2160,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="7">
         <v>1</v>
@@ -2172,10 +2206,10 @@
         <v>4</v>
       </c>
       <c r="O11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2183,10 +2217,10 @@
         <v>102032</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -2210,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="7">
         <v>1</v>
@@ -2222,10 +2256,10 @@
         <v>4</v>
       </c>
       <c r="O12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2233,10 +2267,10 @@
         <v>102033</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
@@ -2272,10 +2306,10 @@
         <v>4</v>
       </c>
       <c r="O13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2283,10 +2317,10 @@
         <v>102041</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
@@ -2322,10 +2356,10 @@
         <v>-5</v>
       </c>
       <c r="O14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2333,10 +2367,10 @@
         <v>102042</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="15">
         <v>1</v>
@@ -2372,10 +2406,10 @@
         <v>-5</v>
       </c>
       <c r="O15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2422,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>37</v>
@@ -2433,10 +2467,10 @@
         <v>103021</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>38</v>
+        <v>269</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>39</v>
+        <v>275</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
@@ -2445,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="9">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="G17" s="9">
         <v>0</v>
@@ -2472,10 +2506,10 @@
         <v>0</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2483,10 +2517,10 @@
         <v>103031</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -2510,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="7">
         <v>1</v>
@@ -2522,10 +2556,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P18" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2533,10 +2567,10 @@
         <v>103032</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
@@ -2560,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="7">
         <v>1</v>
@@ -2572,10 +2606,10 @@
         <v>2</v>
       </c>
       <c r="O19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P19" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2583,10 +2617,10 @@
         <v>103033</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
@@ -2622,10 +2656,10 @@
         <v>2</v>
       </c>
       <c r="O20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P20" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="P20" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2633,10 +2667,10 @@
         <v>103041</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
@@ -2672,10 +2706,10 @@
         <v>-5</v>
       </c>
       <c r="O21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2683,10 +2717,10 @@
         <v>103042</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
@@ -2722,10 +2756,10 @@
         <v>-5</v>
       </c>
       <c r="O22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2736,7 +2770,7 @@
         <v>34</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="18">
         <v>0</v>
@@ -2772,7 +2806,7 @@
         <v>1</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P23" s="17" t="s">
         <v>37</v>
@@ -2783,10 +2817,10 @@
         <v>104021</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>38</v>
+        <v>269</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>39</v>
+        <v>272</v>
       </c>
       <c r="D24" s="9">
         <v>2</v>
@@ -2795,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="9">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="G24" s="9">
         <v>0</v>
@@ -2822,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2833,10 +2867,10 @@
         <v>104031</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="7">
         <v>3</v>
@@ -2872,10 +2906,10 @@
         <v>2</v>
       </c>
       <c r="O25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P25" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2883,10 +2917,10 @@
         <v>104032</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="7">
         <v>3</v>
@@ -2922,10 +2956,10 @@
         <v>2</v>
       </c>
       <c r="O26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P26" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="P26" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2933,10 +2967,10 @@
         <v>104033</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="7">
         <v>3</v>
@@ -2972,10 +3006,10 @@
         <v>2</v>
       </c>
       <c r="O27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P27" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="P27" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2983,10 +3017,10 @@
         <v>104041</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" s="9">
         <v>4</v>
@@ -3007,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="9">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K28" s="9">
         <v>0</v>
@@ -3022,10 +3056,10 @@
         <v>-5</v>
       </c>
       <c r="O28" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P28" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="P28" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -3033,10 +3067,10 @@
         <v>104042</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="9">
         <v>4</v>
@@ -3057,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="9">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="K29" s="9">
         <v>0</v>
@@ -3072,10 +3106,10 @@
         <v>-5</v>
       </c>
       <c r="O29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P29" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -3086,7 +3120,7 @@
         <v>34</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="18">
         <v>0</v>
@@ -3122,7 +3156,7 @@
         <v>1</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P30" s="17" t="s">
         <v>37</v>
@@ -3133,10 +3167,10 @@
         <v>105021</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>38</v>
+        <v>269</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>39</v>
+        <v>271</v>
       </c>
       <c r="D31" s="9">
         <v>2</v>
@@ -3172,10 +3206,10 @@
         <v>0</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P31" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -3183,10 +3217,10 @@
         <v>105031</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="11">
         <v>0</v>
@@ -3222,10 +3256,10 @@
         <v>2</v>
       </c>
       <c r="O32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="P32" s="12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -3233,10 +3267,10 @@
         <v>105032</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" s="11">
         <v>0</v>
@@ -3272,10 +3306,10 @@
         <v>2</v>
       </c>
       <c r="O33" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="P33" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="P33" s="12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -3283,10 +3317,10 @@
         <v>105033</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="11">
         <v>0</v>
@@ -3322,10 +3356,10 @@
         <v>2</v>
       </c>
       <c r="O34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="P34" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -3333,10 +3367,10 @@
         <v>105041</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="7">
         <v>0</v>
@@ -3357,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K35" s="7">
         <v>0</v>
@@ -3372,10 +3406,10 @@
         <v>-5</v>
       </c>
       <c r="O35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P35" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="P35" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3383,10 +3417,10 @@
         <v>105042</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="15">
         <v>0</v>
@@ -3407,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="15">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="K36" s="15">
         <v>0</v>
@@ -3422,10 +3456,10 @@
         <v>-5</v>
       </c>
       <c r="O36" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="P36" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="P36" s="16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3472,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="O37" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P37" s="8" t="s">
         <v>37</v>
@@ -3483,10 +3517,10 @@
         <v>106021</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>38</v>
+        <v>269</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>39</v>
+        <v>276</v>
       </c>
       <c r="D38" s="9">
         <v>2</v>
@@ -3495,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="9">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G38" s="9">
         <v>0</v>
@@ -3522,10 +3556,10 @@
         <v>0</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3533,10 +3567,10 @@
         <v>106031</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="D39" s="7">
         <v>0</v>
@@ -3572,10 +3606,10 @@
         <v>2</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -3583,10 +3617,10 @@
         <v>106032</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="D40" s="7">
         <v>0</v>
@@ -3622,10 +3656,10 @@
         <v>2</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3633,10 +3667,10 @@
         <v>106033</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="D41" s="7">
         <v>0</v>
@@ -3672,10 +3706,10 @@
         <v>2</v>
       </c>
       <c r="O41" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3683,10 +3717,10 @@
         <v>106041</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>95</v>
+        <v>279</v>
       </c>
       <c r="D42" s="7">
         <v>0</v>
@@ -3701,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="I42" s="7">
         <v>0</v>
@@ -3722,10 +3756,10 @@
         <v>-5</v>
       </c>
       <c r="O42" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3733,10 +3767,10 @@
         <v>106042</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>98</v>
+        <v>278</v>
       </c>
       <c r="D43" s="15">
         <v>0</v>
@@ -3751,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="H43" s="15">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="I43" s="15">
         <v>0</v>
@@ -3772,10 +3806,10 @@
         <v>-5</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P43" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3786,7 +3820,7 @@
         <v>34</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D44" s="7">
         <v>0</v>
@@ -3822,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P44" s="8"/>
     </row>
@@ -3831,10 +3865,10 @@
         <v>101001021</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D45" s="20">
         <v>0</v>
@@ -3870,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="P45" s="21"/>
     </row>
@@ -3882,7 +3916,7 @@
         <v>34</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D46" s="7">
         <v>0</v>
@@ -3918,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P46" s="8"/>
     </row>
@@ -3927,10 +3961,10 @@
         <v>101002021</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D47" s="20">
         <v>0</v>
@@ -3966,7 +4000,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P47" s="21"/>
     </row>
@@ -3978,7 +4012,7 @@
         <v>34</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D48" s="7">
         <v>0</v>
@@ -4014,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="O48" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="P48" s="8"/>
     </row>
@@ -4023,10 +4057,10 @@
         <v>101003021</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D49" s="15">
         <v>1</v>
@@ -4062,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P49" s="16"/>
     </row>
@@ -4074,7 +4108,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D50" s="7">
         <v>0</v>
@@ -4110,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P50" s="8"/>
     </row>
@@ -4119,10 +4153,10 @@
         <v>201001021</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D51" s="20">
         <v>1</v>
@@ -4158,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P51" s="21"/>
     </row>
@@ -4170,7 +4204,7 @@
         <v>34</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D52" s="7">
         <v>1</v>
@@ -4206,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P52" s="8"/>
     </row>
@@ -4215,10 +4249,10 @@
         <v>301001021</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D53" s="20">
         <v>0</v>
@@ -4254,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P53" s="21"/>
     </row>
@@ -4290,10 +4324,10 @@
         <v>19</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>30</v>
@@ -4335,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4343,7 +4377,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C4" s="26">
         <v>0</v>
@@ -4358,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4366,7 +4400,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C5" s="26">
         <v>0</v>
@@ -4381,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4389,7 +4423,7 @@
         <v>201</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C6" s="26">
         <v>0</v>
@@ -4404,7 +4438,7 @@
         <v>0.7</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4412,7 +4446,7 @@
         <v>202</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C7" s="26">
         <v>0</v>
@@ -4427,7 +4461,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4435,7 +4469,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C8" s="26">
         <v>0</v>
@@ -4450,7 +4484,7 @@
         <v>0.7</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4458,7 +4492,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -4473,7 +4507,7 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4481,7 +4515,7 @@
         <v>205</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
@@ -4496,7 +4530,7 @@
         <v>0.2</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4504,7 +4538,7 @@
         <v>206</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
@@ -4519,7 +4553,7 @@
         <v>0.3</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
@@ -4527,7 +4561,7 @@
         <v>207</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -4542,7 +4576,7 @@
         <v>0.6</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
@@ -4550,7 +4584,7 @@
         <v>208</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
@@ -4565,7 +4599,7 @@
         <v>0.8</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
@@ -4573,7 +4607,7 @@
         <v>209</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C14" s="26">
         <v>0</v>
@@ -4588,7 +4622,7 @@
         <v>0.9</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4626,43 +4660,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="12.75">
       <c r="A1" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="M1" s="29" t="s">
         <v>145</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="12.75">
@@ -4670,7 +4704,7 @@
         <v>101001</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C2" s="30">
         <v>1</v>
@@ -4700,7 +4734,7 @@
         <v>100</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M2" s="31"/>
     </row>
@@ -4709,7 +4743,7 @@
         <v>101002</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" s="30">
         <v>3</v>
@@ -4739,7 +4773,7 @@
         <v>200</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M3" s="31"/>
     </row>
@@ -4748,7 +4782,7 @@
         <v>101003</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C4" s="30">
         <v>5</v>
@@ -4778,7 +4812,7 @@
         <v>300</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M4" s="31"/>
     </row>
@@ -4787,7 +4821,7 @@
         <v>201001</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5" s="30">
         <v>10</v>
@@ -4817,7 +4851,7 @@
         <v>300</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="M5" s="31"/>
     </row>
@@ -4826,7 +4860,7 @@
         <v>301001</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C6" s="30">
         <v>20</v>
@@ -4856,7 +4890,7 @@
         <v>400</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M6" s="31"/>
     </row>
@@ -4895,49 +4929,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="12.6" customHeight="1">
       <c r="A1" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="33" t="s">
+      <c r="J1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="H1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>145</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>149</v>
       </c>
       <c r="P1" s="33"/>
     </row>
@@ -4946,7 +4980,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" s="33">
         <v>3000</v>
@@ -4982,10 +5016,10 @@
         <v>1.05</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P2" s="35"/>
     </row>
@@ -4994,7 +5028,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C3" s="33">
         <v>2500</v>
@@ -5030,10 +5064,10 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="P3" s="35"/>
     </row>
@@ -5042,7 +5076,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C4" s="33">
         <v>2500</v>
@@ -5078,10 +5112,10 @@
         <v>1.3</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="P4" s="35"/>
     </row>
@@ -5090,7 +5124,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" s="33">
         <v>2000</v>
@@ -5126,10 +5160,10 @@
         <v>1.45</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="P5" s="35"/>
     </row>
@@ -5138,7 +5172,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C6" s="33">
         <v>2000</v>
@@ -5174,10 +5208,10 @@
         <v>1.2</v>
       </c>
       <c r="N6" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="P6" s="35"/>
     </row>
@@ -5186,7 +5220,7 @@
         <v>106</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C7" s="33">
         <v>4000</v>
@@ -5222,10 +5256,10 @@
         <v>0.8</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="P7" s="35"/>
     </row>
@@ -5268,58 +5302,58 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>193</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="P1" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>197</v>
       </c>
       <c r="S1" s="33"/>
     </row>
@@ -5328,7 +5362,7 @@
         <v>110101</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C2" s="33">
         <v>101001</v>
@@ -5369,7 +5403,7 @@
         <v>110102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C3" s="33">
         <v>101001</v>
@@ -5406,7 +5440,7 @@
         <v>110103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C4" s="35">
         <v>101002</v>
@@ -5451,7 +5485,7 @@
         <v>110201</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="35">
         <v>101002</v>
@@ -5483,7 +5517,7 @@
         <v>110202</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C6">
         <v>101002</v>
@@ -5509,7 +5543,7 @@
         <v>110203</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C7">
         <v>101002</v>
@@ -5541,7 +5575,7 @@
         <v>110301</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C8">
         <v>101001</v>
@@ -5567,7 +5601,7 @@
         <v>110302</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C9">
         <v>101001</v>
@@ -5593,7 +5627,7 @@
         <v>110303</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C10">
         <v>101001</v>
@@ -5625,7 +5659,7 @@
         <v>120101</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C11">
         <v>101001</v>
@@ -5651,7 +5685,7 @@
         <v>120102</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C12">
         <v>101001</v>
@@ -5677,7 +5711,7 @@
         <v>120103</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C13">
         <v>101001</v>
@@ -5709,7 +5743,7 @@
         <v>120201</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C14">
         <v>101001</v>
@@ -5735,7 +5769,7 @@
         <v>120202</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C15">
         <v>101001</v>
@@ -5761,7 +5795,7 @@
         <v>120203</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C16">
         <v>101001</v>
@@ -5793,7 +5827,7 @@
         <v>120301</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C17">
         <v>101001</v>
@@ -5819,7 +5853,7 @@
         <v>120302</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C18">
         <v>101001</v>
@@ -5845,7 +5879,7 @@
         <v>120303</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C19">
         <v>101001</v>
@@ -5877,7 +5911,7 @@
         <v>130101</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C20">
         <v>101001</v>
@@ -5903,7 +5937,7 @@
         <v>130102</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C21">
         <v>101001</v>
@@ -5929,7 +5963,7 @@
         <v>130103</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C22">
         <v>101001</v>
@@ -5961,7 +5995,7 @@
         <v>130201</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C23">
         <v>101001</v>
@@ -5987,7 +6021,7 @@
         <v>130202</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C24">
         <v>101001</v>
@@ -6013,7 +6047,7 @@
         <v>130203</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C25">
         <v>101001</v>
@@ -6045,7 +6079,7 @@
         <v>130301</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C26">
         <v>101001</v>
@@ -6071,7 +6105,7 @@
         <v>130302</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C27">
         <v>101001</v>
@@ -6097,7 +6131,7 @@
         <v>130303</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C28">
         <v>101001</v>
@@ -6129,7 +6163,7 @@
         <v>140101</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C29">
         <v>101001</v>
@@ -6155,7 +6189,7 @@
         <v>140102</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C30">
         <v>101001</v>
@@ -6187,7 +6221,7 @@
         <v>140103</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C31">
         <v>101001</v>
@@ -6219,7 +6253,7 @@
         <v>140201</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C32">
         <v>101001</v>
@@ -6245,7 +6279,7 @@
         <v>140202</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C33">
         <v>101001</v>
@@ -6271,7 +6305,7 @@
         <v>140203</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C34">
         <v>101001</v>
@@ -6303,7 +6337,7 @@
         <v>140301</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C35">
         <v>101001</v>
@@ -6329,7 +6363,7 @@
         <v>140302</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C36">
         <v>101001</v>
@@ -6361,7 +6395,7 @@
         <v>140303</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C37">
         <v>101001</v>
@@ -6393,7 +6427,7 @@
         <v>150101</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C38">
         <v>101001</v>
@@ -6419,7 +6453,7 @@
         <v>150102</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C39">
         <v>101001</v>
@@ -6445,7 +6479,7 @@
         <v>150103</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C40">
         <v>101001</v>
@@ -6477,7 +6511,7 @@
         <v>150201</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C41">
         <v>101001</v>
@@ -6503,7 +6537,7 @@
         <v>150202</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C42">
         <v>101001</v>
@@ -6535,7 +6569,7 @@
         <v>150203</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C43">
         <v>101001</v>
@@ -6567,7 +6601,7 @@
         <v>150301</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C44">
         <v>101001</v>
@@ -6593,7 +6627,7 @@
         <v>150302</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C45">
         <v>101001</v>
@@ -6619,7 +6653,7 @@
         <v>150303</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C46">
         <v>101001</v>
@@ -6675,22 +6709,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.5">
       <c r="A1" s="36" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5">
@@ -6698,10 +6732,10 @@
         <v>1101</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D2" s="37">
         <v>110101</v>
@@ -6718,10 +6752,10 @@
         <v>1102</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D3" s="39">
         <v>110201</v>
@@ -6738,10 +6772,10 @@
         <v>1103</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D4" s="39">
         <v>110301</v>
@@ -6758,10 +6792,10 @@
         <v>1201</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D5" s="37">
         <v>120101</v>
@@ -6778,10 +6812,10 @@
         <v>1202</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D6" s="39">
         <v>120201</v>
@@ -6798,10 +6832,10 @@
         <v>1203</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D7" s="39">
         <v>120301</v>
@@ -6818,10 +6852,10 @@
         <v>1301</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D8" s="37">
         <v>130101</v>
@@ -6838,10 +6872,10 @@
         <v>1302</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D9" s="39">
         <v>130201</v>
@@ -6858,10 +6892,10 @@
         <v>1303</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D10" s="39">
         <v>130301</v>
@@ -6878,10 +6912,10 @@
         <v>1401</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D11" s="37">
         <v>140101</v>
@@ -6898,10 +6932,10 @@
         <v>1402</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D12" s="39">
         <v>140201</v>
@@ -6918,10 +6952,10 @@
         <v>1403</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D13" s="39">
         <v>140301</v>
@@ -6938,10 +6972,10 @@
         <v>1501</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D14" s="37">
         <v>150101</v>
@@ -6958,10 +6992,10 @@
         <v>1502</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D15" s="39">
         <v>150201</v>
@@ -6978,10 +7012,10 @@
         <v>1503</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D16" s="39">
         <v>150301</v>
@@ -6998,10 +7032,10 @@
         <v>1601</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D17" s="37">
         <v>160101</v>
@@ -7018,10 +7052,10 @@
         <v>1602</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D18" s="37">
         <v>160201</v>
@@ -7038,10 +7072,10 @@
         <v>1603</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D19" s="37">
         <v>160301</v>
@@ -7081,25 +7115,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24">
       <c r="A1" s="33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24">
@@ -7107,13 +7141,13 @@
         <v>10101</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E2" s="33">
         <v>20</v>
@@ -7122,7 +7156,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24">
@@ -7130,13 +7164,13 @@
         <v>10102</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E3" s="33">
         <v>50</v>
@@ -7145,7 +7179,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24">
@@ -7153,13 +7187,13 @@
         <v>10103</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E4" s="33">
         <v>100</v>
@@ -7168,7 +7202,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24">
@@ -7176,13 +7210,13 @@
         <v>10201</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
@@ -7191,7 +7225,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24">
@@ -7199,13 +7233,13 @@
         <v>10301</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E6" s="33">
         <v>1</v>
@@ -7214,7 +7248,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24">
@@ -7222,13 +7256,13 @@
         <v>10401</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E7" s="33">
         <v>50</v>
@@ -7237,7 +7271,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24">
@@ -7245,13 +7279,13 @@
         <v>10402</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E8" s="33">
         <v>150</v>
@@ -7260,7 +7294,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7268,13 +7302,13 @@
         <v>10501</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E9" s="33">
         <v>1</v>
@@ -7283,7 +7317,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7291,13 +7325,13 @@
         <v>10601</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E10" s="33">
         <v>101</v>
@@ -7306,7 +7340,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7314,13 +7348,13 @@
         <v>10602</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E11" s="33">
         <v>102</v>
@@ -7329,7 +7363,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7337,13 +7371,13 @@
         <v>10603</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E12" s="33">
         <v>103</v>
@@ -7352,7 +7386,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7360,13 +7394,13 @@
         <v>10604</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E13" s="33">
         <v>104</v>
@@ -7375,7 +7409,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -7383,13 +7417,13 @@
         <v>10605</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E14" s="33">
         <v>105</v>
@@ -7398,7 +7432,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -7406,13 +7440,13 @@
         <v>10606</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E15" s="33">
         <v>106</v>
@@ -7421,7 +7455,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -7429,10 +7463,10 @@
         <v>10701</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -7464,10 +7498,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>